<commit_message>
ann qf605 project part2 fix calibr fail
</commit_message>
<xml_diff>
--- a/qf605-fixed-income/ann/data/model_calibration.xlsx
+++ b/qf605-fixed-income/ann/data/model_calibration.xlsx
@@ -555,19 +555,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1.695348069761121e-11</v>
+        <v>7.885246997224849e-12</v>
       </c>
       <c r="C2" t="n">
-        <v>4.789389593976652e-12</v>
+        <v>6.962226877467228e-07</v>
       </c>
       <c r="D2" t="n">
-        <v>5.454215528370767e-06</v>
+        <v>3.832329636968492e-09</v>
       </c>
       <c r="E2" t="n">
-        <v>3.224735843298715e-06</v>
+        <v>9.471907038297822e-07</v>
       </c>
       <c r="F2" t="n">
-        <v>2.200213444201148e-05</v>
+        <v>4.751541411568416e-05</v>
       </c>
     </row>
     <row r="3">
@@ -575,19 +575,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.893195248418145e-06</v>
+        <v>1.608894123934842e-07</v>
       </c>
       <c r="C3" t="n">
-        <v>1.088217716799125e-07</v>
+        <v>3.552976753402209e-08</v>
       </c>
       <c r="D3" t="n">
-        <v>1.090821218942273e-06</v>
+        <v>1.096232868399549e-07</v>
       </c>
       <c r="E3" t="n">
-        <v>1.648764770530078e-05</v>
+        <v>4.023029195069023e-07</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05785894977242365</v>
+        <v>0.04709860625464218</v>
       </c>
     </row>
     <row r="4">
@@ -595,19 +595,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>1.886394933426445e-07</v>
+        <v>4.614165728620829e-08</v>
       </c>
       <c r="C4" t="n">
-        <v>2.426600724548698e-06</v>
+        <v>1.652261114429331e-07</v>
       </c>
       <c r="D4" t="n">
-        <v>1.371611962273011e-05</v>
+        <v>4.184802500863572e-07</v>
       </c>
       <c r="E4" t="n">
-        <v>6.468376793835901e-05</v>
+        <v>1.030430094713379e-06</v>
       </c>
       <c r="F4" t="n">
-        <v>0.005125829600431474</v>
+        <v>0.0004840579107775311</v>
       </c>
     </row>
   </sheetData>
@@ -651,19 +651,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1466476407283374</v>
+        <v>0.1390684910679972</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1892971483471333</v>
+        <v>0.1846468872735449</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2027010309137504</v>
+        <v>0.1968590050369231</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1821933541981159</v>
+        <v>0.1781924798299023</v>
       </c>
       <c r="F2" t="n">
-        <v>0.172925431367198</v>
+        <v>0.1730826076136539</v>
       </c>
     </row>
     <row r="3">
@@ -671,19 +671,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1624482582385495</v>
+        <v>0.1666187379290287</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1957968569479028</v>
+        <v>0.199448782766367</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2036049417546076</v>
+        <v>0.2099652199571752</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1768998645644443</v>
+        <v>0.1893675389833352</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1615384073961845</v>
+        <v>0.1721029611474361</v>
       </c>
     </row>
     <row r="4">
@@ -691,19 +691,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1638478194170534</v>
+        <v>0.1783349764874097</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1751259714147292</v>
+        <v>0.1965869454748382</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1805536991780063</v>
+        <v>0.2088713195118277</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1639850929638545</v>
+        <v>0.2024122688382498</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1492184043241639</v>
+        <v>0.1799196486984244</v>
       </c>
     </row>
   </sheetData>
@@ -747,19 +747,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.6080119350612362</v>
+        <v>-0.6332311314898889</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.5247468489355788</v>
+        <v>-0.5251222516691815</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4926640159093795</v>
+        <v>-0.4829285887755333</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.4269030831672759</v>
+        <v>-0.4164267051937015</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.2535367993446147</v>
+        <v>-0.3104438248351558</v>
       </c>
     </row>
     <row r="3">
@@ -767,19 +767,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.5497352854209429</v>
+        <v>-0.585702216395778</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.5207455875877792</v>
+        <v>-0.5467500857417683</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5146381508216121</v>
+        <v>-0.5484175077637466</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.3941735933207814</v>
+        <v>-0.50465255201821</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2478408401476662</v>
+        <v>-0.4058151147306712</v>
       </c>
     </row>
     <row r="4">
@@ -787,19 +787,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4788956883653683</v>
+        <v>-0.5485894990962054</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4633799232510829</v>
+        <v>-0.5482504621442114</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4471050330251283</v>
+        <v>-0.5550633393882645</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.3798048737278831</v>
+        <v>-0.5673076703967784</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2536222578777956</v>
+        <v>-0.5161195528555906</v>
       </c>
     </row>
   </sheetData>
@@ -843,19 +843,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1.930101030848361</v>
+        <v>2.049504410648026</v>
       </c>
       <c r="C2" t="n">
-        <v>1.627065353184448</v>
+        <v>1.677435845505478</v>
       </c>
       <c r="D2" t="n">
-        <v>1.387246101440456</v>
+        <v>1.438149895111271</v>
       </c>
       <c r="E2" t="n">
-        <v>1.021621793588593</v>
+        <v>1.064294097686372</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7503968555263733</v>
+        <v>0.7580449319019704</v>
       </c>
     </row>
     <row r="3">
@@ -863,19 +863,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.281969189513937</v>
+        <v>1.34052141303805</v>
       </c>
       <c r="C3" t="n">
-        <v>1.034017309371821</v>
+        <v>1.061949312765889</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9169750633427028</v>
+        <v>0.9366376306559135</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6950684493174126</v>
+        <v>0.6809826811980543</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5653576233502046</v>
+        <v>0.5396187621252914</v>
       </c>
     </row>
     <row r="4">
@@ -883,19 +883,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9440770695684426</v>
+        <v>1.010440516131548</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8640968834856623</v>
+        <v>0.9292667123447461</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8060949706218881</v>
+        <v>0.8729728280510581</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6828272036005124</v>
+        <v>0.7282767050467239</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5909471648417995</v>
+        <v>0.5989356093636879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>